<commit_message>
maj Title, description, minification js, balise semantique,lang fr, errors html/css and include meta robot
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -62,12 +62,13 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">accessiblité</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">mettre un titre qui correspond a la nature du site</t>
+    <t xml:space="preserve">mettre un titre qui correspond a la ste ou nature du site</t>
   </si>
   <si>
     <t xml:space="preserve">script en début </t>
@@ -76,7 +77,7 @@
     <t xml:space="preserve">mettre le script en fin pour fluidifier le chargement</t>
   </si>
   <si>
-    <t xml:space="preserve">mettre le script en fin afin que les scripte ne gêne pas le chargement de la page</t>
+    <t xml:space="preserve">mettre le script en fin afin que les scripts ne gêne pas le chargement de la page</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -112,15 +113,6 @@
     <t xml:space="preserve">ajouter une description donnant la nature du site</t>
   </si>
   <si>
-    <t xml:space="preserve">indentation html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">faciliter la lecture html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mettre à jour le code HTML</t>
-  </si>
-  <si>
     <t xml:space="preserve">lien mal indiquer </t>
   </si>
   <si>
@@ -188,6 +180,24 @@
   </si>
   <si>
     <t xml:space="preserve">1 erreur lang par defaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Style inclus dans le HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style dans des balises html  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inclure dans le style.css </t>
+  </si>
+  <si>
+    <t xml:space="preserve">black hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">texte invisible page 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l’afficher en visible</t>
   </si>
 </sst>
 </file>
@@ -197,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -241,19 +251,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -331,11 +335,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,8 +347,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -424,19 +428,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="62.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="52.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
   </cols>
@@ -559,8 +562,8 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
+      <c r="A7" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>24</v>
@@ -571,7 +574,7 @@
       <c r="D7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
@@ -586,11 +589,11 @@
       <c r="D8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>30</v>
@@ -605,7 +608,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>33</v>
@@ -616,7 +619,7 @@
       <c r="D10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
@@ -631,7 +634,7 @@
       <c r="D11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
@@ -640,13 +643,13 @@
       <c r="B12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -674,28 +677,38 @@
         <v>46</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
@@ -710,7 +723,6 @@
       <c r="B19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
       <c r="B20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -755,9 +767,7 @@
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="4"/>
-    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1722,7 +1732,7 @@
     <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
maj audit + page 2 and correction color /police AA du WCAG 2.1
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -191,13 +191,31 @@
     <t xml:space="preserve">inclure dans le style.css </t>
   </si>
   <si>
-    <t xml:space="preserve">black hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">texte invisible page 2</t>
+    <t xml:space="preserve">Texte invisible page 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">texte non lisible par l’utilisateur</t>
   </si>
   <si>
     <t xml:space="preserve">l’afficher en visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessiblité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur non conforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couleur non conforme au norme  du niveau AA du WCAG 2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correction des couleurs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">police trop petite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">police trop petite sur certain texte</t>
   </si>
 </sst>
 </file>
@@ -207,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -258,6 +276,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -314,7 +338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -349,6 +373,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -431,7 +459,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,46 +739,74 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="4"/>

</xml_diff>

<commit_message>
maj audit and add focus
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nita\Desktop\Formation\Livrable projet 4\Starting website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C34DB3-FB45-4BCC-9BED-739A2DAFEBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65BD059-AC91-40E7-8252-242281018784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>Catégorie</t>
   </si>
@@ -236,12 +236,6 @@
     <t>favorise un crowling fluide (cohérence lors de l'exploration google)</t>
   </si>
   <si>
-    <t>10 erreurs trouvées (principalement des erreurs de code non fonctionnel)</t>
-  </si>
-  <si>
-    <t>1 erreur lang par defaut ( il faut indiquer la lanque du pays concerné)</t>
-  </si>
-  <si>
     <t>style dans des balises html  (pas recommandé)</t>
   </si>
   <si>
@@ -276,6 +270,25 @@
   </si>
   <si>
     <t>https://josselinleydier.com/seo/texte-cache-seo/</t>
+  </si>
+  <si>
+    <t>Pas de focus visible</t>
+  </si>
+  <si>
+    <t>Pas de focus visible lors de la navigation avec le clavier</t>
+  </si>
+  <si>
+    <t>Penser au utilisateur explorant le site au clavier</t>
+  </si>
+  <si>
+    <t>8 erreurs trouvées (principalement des erreurs de code non fonctionnel)</t>
+  </si>
+  <si>
+    <t>1 erreur lang par defaut 
+3 erreurs trouvées (principalement des erreurs de code non fonctionnel) page2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indiquer la lanque du pays concerné permet a google de mieux ce situer et idem pour les logiciéls d'accessibilités </t>
   </si>
 </sst>
 </file>
@@ -755,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,7 +1038,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>40</v>
@@ -1043,10 +1056,10 @@
         <v>41</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="9" t="s">
@@ -1061,7 +1074,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>43</v>
@@ -1079,7 +1092,7 @@
         <v>44</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>45</v>
@@ -1112,17 +1125,17 @@
         <v>13</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1130,43 +1143,57 @@
         <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>50</v>
+      <c r="B20" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="E20" s="15"/>
       <c r="F20" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+    <row r="21" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
@@ -1208,6 +1235,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
@@ -1221,7 +1249,9 @@
     <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2186,6 +2216,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2195,7 +2226,7 @@
     <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="F17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="F19" r:id="rId9" xr:uid="{96952504-961A-4F82-BD65-1C74543E2992}"/>
     <hyperlink ref="F18" r:id="rId10" xr:uid="{0E148952-A709-4993-99AB-E6B12A57192E}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
change image to text
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nita\Desktop\Formation\Livrable projet 4\Starting website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D61418-E1EE-4A89-897D-88E62E8416DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AFCFDF-60C2-46E6-9A14-F4CBAB6883F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>Catégorie</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>Police trop petite sur certain texte cause des complications pour l'accessibilité de tous</t>
+  </si>
+  <si>
+    <t>Image en texte</t>
+  </si>
+  <si>
+    <t>Certains textes dans l'index sont en images</t>
+  </si>
+  <si>
+    <t>Afficher le texte en texte brute</t>
   </si>
 </sst>
 </file>
@@ -389,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,6 +444,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -785,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,35 +992,35 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>76</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9" t="s">
-        <v>20</v>
+        <v>78</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="11" t="s">
-        <v>21</v>
+        <v>54</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1016,107 +1028,107 @@
         <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="9" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>12</v>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="10" t="s">
-        <v>23</v>
+        <v>65</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="13"/>
       <c r="F15" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>31</v>
+        <v>69</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>13</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1124,35 +1136,35 @@
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1160,25 +1172,39 @@
         <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E19" s="15"/>
       <c r="F19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+    <row r="20" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
@@ -1220,6 +1246,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
@@ -1233,7 +1260,9 @@
     <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2198,6 +2227,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2205,11 +2235,11 @@
     <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F17" r:id="rId9" xr:uid="{96952504-961A-4F82-BD65-1C74543E2992}"/>
-    <hyperlink ref="F16" r:id="rId10" xr:uid="{0E148952-A709-4993-99AB-E6B12A57192E}"/>
+    <hyperlink ref="F15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{96952504-961A-4F82-BD65-1C74543E2992}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{0E148952-A709-4993-99AB-E6B12A57192E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>

</xml_diff>